<commit_message>
Added validation results to output
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\lrcfs-electron-file-renamer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E65A2B0-9914-453F-A54C-9A1450FE5769}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486519A4-125D-467F-951A-E299A8E3505A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39900" yWindow="1210" windowWidth="26750" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45100" yWindow="4520" windowWidth="21580" windowHeight="13840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -75,12 +75,6 @@
     <t>002</t>
   </si>
   <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
     <t>ObsType</t>
   </si>
   <si>
@@ -126,28 +120,13 @@
     <t>Nylo01</t>
   </si>
   <si>
-    <t>A01</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
     <t>IMG_002.JPG</t>
   </si>
   <si>
-    <t>IMG_003.JPG</t>
-  </si>
-  <si>
-    <t>IMG_004.JPG</t>
-  </si>
-  <si>
     <t>OriginalFilename</t>
-  </si>
-  <si>
-    <t>missing.jpg</t>
   </si>
 </sst>
 </file>
@@ -570,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T121"/>
+  <dimension ref="A1:T115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,7 +567,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -603,37 +582,37 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
@@ -663,19 +642,19 @@
         <v>8</v>
       </c>
       <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -685,12 +664,12 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>20190828</v>
@@ -712,283 +691,151 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
         <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>IF(I3="NA",0,IF(OR(I3="A01",I3="A02",I3="A03",I3="A04"),60,IF(I3="A05",30,IF(I3="A06",120,IF(I3="A07",240,Error)))))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>20190828</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <f>IF(I4="NA",0,IF(OR(I4="A01",I4="A02",I4="A03",I4="A04"),60,IF(I4="A05",30,IF(I4="A06",120,IF(I4="A07",240,Error)))))</f>
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>20190828</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <f>IF(I5="NA",0,IF(OR(I5="A01",I5="A05",I5="A06",I5="A07"),1000,IF(I5="A02",700,IF(I5="A03",500,IF(I5="A04",200,Error)))))</f>
-        <v>1000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5">
-        <v>216</v>
-      </c>
-      <c r="Q5">
-        <f>IF(I5="NA",0,IF(OR(I5="A01",I5="A02",I5="A03",I5="A04"),60,IF(I5="A05",30,IF(I5="A06",120,IF(I5="A07",240,Error)))))</f>
-        <v>60</v>
-      </c>
-      <c r="R5" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6">
-        <v>20190828</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <f>IF(I6="NA",0,IF(OR(I6="A01",I6="A05",I6="A06",I6="A07"),1000,IF(I6="A02",700,IF(I6="A03",500,IF(I6="A04",200,Error)))))</f>
-        <v>1000</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6">
-        <v>139</v>
-      </c>
-      <c r="Q6">
-        <f>IF(I6="NA",0,IF(OR(I6="A01",I6="A02",I6="A03",I6="A04"),60,IF(I6="A05",30,IF(I6="A06",120,IF(I6="A07",240,Error)))))</f>
-        <v>60</v>
-      </c>
-      <c r="R6" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>20190828</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <f>IF(I7="NA",0,IF(OR(I7="A01",I7="A05",I7="A06",I7="A07"),1000,IF(I7="A02",700,IF(I7="A03",500,IF(I7="A04",200,Error)))))</f>
-        <v>1000</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7">
-        <v>139</v>
-      </c>
-      <c r="Q7">
-        <f>IF(I7="NA",0,IF(OR(I7="A01",I7="A02",I7="A03",I7="A04"),60,IF(I7="A05",30,IF(I7="A06",120,IF(I7="A07",240,Error)))))</f>
-        <v>60</v>
-      </c>
-      <c r="R7" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q7"/>
+      <c r="R7"/>
       <c r="S7"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="1"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="1"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -1006,9 +853,6 @@
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -1022,7 +866,7 @@
       <c r="S16" s="9"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1036,7 +880,7 @@
       <c r="S17" s="9"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1050,7 +894,7 @@
       <c r="S18" s="9"/>
       <c r="T18" s="6"/>
     </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1064,7 +908,7 @@
       <c r="S19" s="9"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1078,7 +922,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="6"/>
     </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -1092,7 +936,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -1106,7 +950,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1120,7 +964,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
@@ -1134,7 +978,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1148,7 +992,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1162,7 +1006,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="6"/>
     </row>
-    <row r="27" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -1176,7 +1020,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -1190,7 +1034,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1204,7 +1048,8 @@
       <c r="S29" s="9"/>
       <c r="T29" s="6"/>
     </row>
-    <row r="30" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:20" x14ac:dyDescent="0.35">
+      <c r="D30" s="5"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -1218,7 +1063,8 @@
       <c r="S30" s="9"/>
       <c r="T30" s="6"/>
     </row>
-    <row r="31" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:20" x14ac:dyDescent="0.35">
+      <c r="D31" s="5"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1232,7 +1078,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="9:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:20" x14ac:dyDescent="0.35">
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -1246,7 +1092,7 @@
       <c r="S32" s="9"/>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -1260,7 +1106,7 @@
       <c r="S33" s="9"/>
       <c r="T33" s="6"/>
     </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -1274,7 +1120,7 @@
       <c r="S34" s="9"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -1288,8 +1134,7 @@
       <c r="S35" s="9"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="4:20" x14ac:dyDescent="0.35">
-      <c r="D36" s="5"/>
+    <row r="36" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -1303,8 +1148,7 @@
       <c r="S36" s="9"/>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="4:20" x14ac:dyDescent="0.35">
-      <c r="D37" s="5"/>
+    <row r="37" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -1318,7 +1162,7 @@
       <c r="S37" s="9"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -1332,7 +1176,7 @@
       <c r="S38" s="9"/>
       <c r="T38" s="6"/>
     </row>
-    <row r="39" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -1346,7 +1190,7 @@
       <c r="S39" s="9"/>
       <c r="T39" s="6"/>
     </row>
-    <row r="40" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -1360,7 +1204,7 @@
       <c r="S40" s="9"/>
       <c r="T40" s="6"/>
     </row>
-    <row r="41" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -1374,7 +1218,7 @@
       <c r="S41" s="9"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
@@ -1388,7 +1232,7 @@
       <c r="S42" s="9"/>
       <c r="T42" s="6"/>
     </row>
-    <row r="43" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -1402,7 +1246,7 @@
       <c r="S43" s="9"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -1416,7 +1260,7 @@
       <c r="S44" s="9"/>
       <c r="T44" s="6"/>
     </row>
-    <row r="45" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -1430,7 +1274,7 @@
       <c r="S45" s="9"/>
       <c r="T45" s="6"/>
     </row>
-    <row r="46" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -1444,7 +1288,7 @@
       <c r="S46" s="9"/>
       <c r="T46" s="6"/>
     </row>
-    <row r="47" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -1458,7 +1302,7 @@
       <c r="S47" s="9"/>
       <c r="T47" s="6"/>
     </row>
-    <row r="48" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="9:20" x14ac:dyDescent="0.35">
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -2397,102 +2241,18 @@
       <c r="T114" s="6"/>
     </row>
     <row r="115" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I115" s="6"/>
-      <c r="J115" s="6"/>
-      <c r="K115" s="6"/>
-      <c r="L115" s="6"/>
-      <c r="M115" s="6"/>
-      <c r="N115" s="6"/>
-      <c r="O115" s="6"/>
-      <c r="P115" s="6"/>
-      <c r="Q115" s="7"/>
-      <c r="R115" s="8"/>
-      <c r="S115" s="9"/>
-      <c r="T115" s="6"/>
-    </row>
-    <row r="116" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I116" s="6"/>
-      <c r="J116" s="6"/>
-      <c r="K116" s="6"/>
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
-      <c r="N116" s="6"/>
-      <c r="O116" s="6"/>
-      <c r="P116" s="6"/>
-      <c r="Q116" s="7"/>
-      <c r="R116" s="8"/>
-      <c r="S116" s="9"/>
-      <c r="T116" s="6"/>
-    </row>
-    <row r="117" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I117" s="6"/>
-      <c r="J117" s="6"/>
-      <c r="K117" s="6"/>
-      <c r="L117" s="6"/>
-      <c r="M117" s="6"/>
-      <c r="N117" s="6"/>
-      <c r="O117" s="6"/>
-      <c r="P117" s="6"/>
-      <c r="Q117" s="7"/>
-      <c r="R117" s="8"/>
-      <c r="S117" s="9"/>
-      <c r="T117" s="6"/>
-    </row>
-    <row r="118" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I118" s="6"/>
-      <c r="J118" s="6"/>
-      <c r="K118" s="6"/>
-      <c r="L118" s="6"/>
-      <c r="M118" s="6"/>
-      <c r="N118" s="6"/>
-      <c r="O118" s="6"/>
-      <c r="P118" s="6"/>
-      <c r="Q118" s="7"/>
-      <c r="R118" s="8"/>
-      <c r="S118" s="9"/>
-      <c r="T118" s="6"/>
-    </row>
-    <row r="119" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I119" s="6"/>
-      <c r="J119" s="6"/>
-      <c r="K119" s="6"/>
-      <c r="L119" s="6"/>
-      <c r="M119" s="6"/>
-      <c r="N119" s="6"/>
-      <c r="O119" s="6"/>
-      <c r="P119" s="6"/>
-      <c r="Q119" s="7"/>
-      <c r="R119" s="8"/>
-      <c r="S119" s="9"/>
-      <c r="T119" s="6"/>
-    </row>
-    <row r="120" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I120" s="6"/>
-      <c r="J120" s="6"/>
-      <c r="K120" s="6"/>
-      <c r="L120" s="6"/>
-      <c r="M120" s="6"/>
-      <c r="N120" s="6"/>
-      <c r="O120" s="6"/>
-      <c r="P120" s="6"/>
-      <c r="Q120" s="7"/>
-      <c r="R120" s="8"/>
-      <c r="S120" s="9"/>
-      <c r="T120" s="6"/>
-    </row>
-    <row r="121" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I121" s="10"/>
-      <c r="J121" s="10"/>
-      <c r="K121" s="10"/>
-      <c r="L121" s="10"/>
-      <c r="M121" s="10"/>
-      <c r="N121" s="10"/>
-      <c r="O121" s="10"/>
-      <c r="P121" s="10"/>
-      <c r="Q121" s="11"/>
-      <c r="R121" s="12"/>
-      <c r="S121" s="13"/>
-      <c r="T121" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="J115" s="10"/>
+      <c r="K115" s="10"/>
+      <c r="L115" s="10"/>
+      <c r="M115" s="10"/>
+      <c r="N115" s="10"/>
+      <c r="O115" s="10"/>
+      <c r="P115" s="10"/>
+      <c r="Q115" s="11"/>
+      <c r="R115" s="12"/>
+      <c r="S115" s="13"/>
+      <c r="T115" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>